<commit_message>
changes to reflect minor post vote corrections by office
</commit_message>
<xml_diff>
--- a/budget_2023.xlsx
+++ b/budget_2023.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\01_Dave\Programs\GitHub_home\budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D230763-F200-465A-A413-6E44E1C6B58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F74E2D-D102-400C-B306-B90717F7491F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17925" yWindow="0" windowWidth="10980" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2003 budget" sheetId="7" r:id="rId1"/>
@@ -21,13 +21,13 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2003 budget'!$A$1:$S$204</definedName>
-    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable2" hidden="1">'[1]budget 11-01-23'!$A$1:$M$198</definedName>
-    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable3" hidden="1">Table1</definedName>
+    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable21" hidden="1">'[1]budget 11-01-23'!$A$1:$M$198</definedName>
+    <definedName name="_xlcn.WorksheetConnection_budget_2024.xlsxTable31" hidden="1">Table1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2003 budget'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
@@ -100,7 +100,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table2" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable2"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable21"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -109,7 +109,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Table3">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable3"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_budget_2024.xlsxTable31"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="294">
   <si>
     <t>Recurring or 1-time Expense</t>
   </si>
@@ -994,6 +994,12 @@
   </si>
   <si>
     <t>Budget</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Out</t>
   </si>
 </sst>
 </file>
@@ -1146,16 +1152,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6F80153F-CDA1-4E91-9FDD-43E3E0555995}"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     </dxf>
@@ -4967,7 +4964,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A4E7FDD-FE94-45A4-A7AC-6A49F24B5877}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A4E7FDD-FE94-45A4-A7AC-6A49F24B5877}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:C32" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0">
@@ -5140,7 +5137,7 @@
     <dataField name="Sum of 2023 Budget 4/4/23" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -5359,10 +5356,10 @@
   </sheetPr>
   <dimension ref="A1:Q204"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L17" sqref="L17"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27:A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5436,7 +5433,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -5479,7 +5476,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -5522,7 +5519,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -5565,7 +5562,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -5608,7 +5605,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -5651,7 +5648,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -5694,7 +5691,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -5737,7 +5734,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -5780,7 +5777,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>28</v>
@@ -5823,7 +5820,7 @@
     </row>
     <row r="11" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
@@ -5857,7 +5854,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>28</v>
@@ -5900,7 +5897,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
@@ -5946,7 +5943,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
@@ -5989,7 +5986,7 @@
     </row>
     <row r="15" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>282</v>
@@ -6035,7 +6032,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>282</v>
@@ -6081,7 +6078,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>282</v>
@@ -6124,7 +6121,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>282</v>
@@ -6167,7 +6164,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>282</v>
@@ -6210,7 +6207,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>282</v>
@@ -6256,7 +6253,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>31</v>
@@ -6299,7 +6296,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
@@ -6342,7 +6339,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>31</v>
@@ -6385,7 +6382,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>31</v>
@@ -6428,7 +6425,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>31</v>
@@ -6474,7 +6471,7 @@
     </row>
     <row r="26" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>3</v>
+        <v>292</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>31</v>
@@ -6508,7 +6505,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>181</v>
@@ -6551,7 +6548,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>181</v>
@@ -6597,7 +6594,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>181</v>
@@ -6640,7 +6637,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>181</v>
@@ -6683,7 +6680,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>181</v>
@@ -6726,7 +6723,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>181</v>
@@ -6769,7 +6766,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>181</v>
@@ -6812,7 +6809,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>181</v>
@@ -6855,7 +6852,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>181</v>
@@ -6898,7 +6895,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>181</v>
@@ -6941,7 +6938,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>181</v>
@@ -6984,7 +6981,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>181</v>
@@ -7027,7 +7024,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>181</v>
@@ -7070,7 +7067,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>193</v>
@@ -7113,7 +7110,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>193</v>
@@ -7159,7 +7156,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>193</v>
@@ -7202,7 +7199,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>193</v>
@@ -7245,7 +7242,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>193</v>
@@ -7288,7 +7285,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>102</v>
@@ -7331,7 +7328,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>102</v>
@@ -7374,7 +7371,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>102</v>
@@ -7417,7 +7414,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>102</v>
@@ -7460,7 +7457,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>102</v>
@@ -7503,7 +7500,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>102</v>
@@ -7546,7 +7543,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>179</v>
@@ -7589,7 +7586,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>179</v>
@@ -7632,7 +7629,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>179</v>
@@ -7675,7 +7672,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>112</v>
@@ -7718,7 +7715,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>112</v>
@@ -7761,7 +7758,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>112</v>
@@ -7804,7 +7801,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>112</v>
@@ -7847,7 +7844,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>112</v>
@@ -7890,7 +7887,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>117</v>
@@ -7933,7 +7930,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>117</v>
@@ -7979,7 +7976,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>117</v>
@@ -8022,7 +8019,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>117</v>
@@ -8065,7 +8062,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>117</v>
@@ -8108,7 +8105,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>117</v>
@@ -8151,7 +8148,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>117</v>
@@ -8197,7 +8194,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>117</v>
@@ -8240,7 +8237,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>199</v>
@@ -8283,7 +8280,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>199</v>
@@ -8326,7 +8323,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>199</v>
@@ -8369,7 +8366,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>199</v>
@@ -8412,7 +8409,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>199</v>
@@ -8455,7 +8452,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>199</v>
@@ -8498,7 +8495,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>205</v>
@@ -8544,7 +8541,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>205</v>
@@ -8587,7 +8584,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>205</v>
@@ -8630,7 +8627,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>205</v>
@@ -8673,7 +8670,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>15</v>
@@ -8716,7 +8713,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>94</v>
@@ -8759,7 +8756,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>132</v>
@@ -8802,7 +8799,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>132</v>
@@ -8845,7 +8842,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>132</v>
@@ -8888,7 +8885,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>132</v>
@@ -8931,7 +8928,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
@@ -8974,7 +8971,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>
@@ -9017,7 +9014,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>4</v>
@@ -9060,7 +9057,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>4</v>
@@ -9103,7 +9100,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>4</v>
@@ -9146,7 +9143,7 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
@@ -9189,7 +9186,7 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>4</v>
@@ -9232,7 +9229,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>4</v>
@@ -9275,7 +9272,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>4</v>
@@ -9318,7 +9315,7 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>108</v>
@@ -9361,7 +9358,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>108</v>
@@ -9404,7 +9401,7 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>108</v>
@@ -9447,7 +9444,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>108</v>
@@ -9490,7 +9487,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>14</v>
@@ -9533,7 +9530,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>14</v>
@@ -9576,7 +9573,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>14</v>
@@ -9619,7 +9616,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>14</v>
@@ -9662,7 +9659,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>14</v>
@@ -9705,7 +9702,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>14</v>
@@ -9748,7 +9745,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>14</v>
@@ -9791,7 +9788,7 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>14</v>
@@ -9834,7 +9831,7 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>14</v>
@@ -9877,7 +9874,7 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>14</v>
@@ -9920,7 +9917,7 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>127</v>
@@ -9963,7 +9960,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>127</v>
@@ -10006,7 +10003,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>127</v>
@@ -10052,7 +10049,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>127</v>
@@ -10098,7 +10095,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>97</v>
@@ -10141,7 +10138,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>97</v>
@@ -10184,7 +10181,7 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>97</v>
@@ -10227,7 +10224,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>97</v>
@@ -10270,7 +10267,7 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>100</v>
@@ -10316,7 +10313,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>100</v>
@@ -10359,7 +10356,7 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>136</v>
@@ -10402,7 +10399,7 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>136</v>
@@ -10445,7 +10442,7 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>136</v>
@@ -10488,7 +10485,7 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>136</v>
@@ -10531,7 +10528,7 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>136</v>
@@ -10574,7 +10571,7 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>136</v>
@@ -10617,7 +10614,7 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>136</v>
@@ -10660,7 +10657,7 @@
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>136</v>
@@ -10703,7 +10700,7 @@
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>136</v>
@@ -10746,7 +10743,7 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>136</v>
@@ -10789,7 +10786,7 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>136</v>
@@ -10832,7 +10829,7 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>136</v>
@@ -10875,7 +10872,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>136</v>
@@ -10918,7 +10915,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>136</v>
@@ -10961,7 +10958,7 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>136</v>
@@ -11004,7 +11001,7 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>136</v>
@@ -11047,7 +11044,7 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>136</v>
@@ -11090,7 +11087,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>136</v>
@@ -11133,7 +11130,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>136</v>
@@ -11176,7 +11173,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>136</v>
@@ -11219,7 +11216,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>136</v>
@@ -11262,7 +11259,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>136</v>
@@ -11305,7 +11302,7 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>136</v>
@@ -11348,7 +11345,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>136</v>
@@ -11391,7 +11388,7 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>136</v>
@@ -11434,7 +11431,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>136</v>
@@ -11477,7 +11474,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>136</v>
@@ -11520,7 +11517,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>136</v>
@@ -11563,7 +11560,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>163</v>
@@ -11606,7 +11603,7 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>163</v>
@@ -11652,7 +11649,7 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>163</v>
@@ -11695,7 +11692,7 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>163</v>
@@ -11738,7 +11735,7 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>163</v>
@@ -11781,7 +11778,7 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>39</v>
@@ -11824,7 +11821,7 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>39</v>
@@ -11867,7 +11864,7 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>39</v>
@@ -11910,7 +11907,7 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>39</v>
@@ -11953,7 +11950,7 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>39</v>
@@ -11996,7 +11993,7 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>39</v>
@@ -12039,7 +12036,7 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>39</v>
@@ -12082,7 +12079,7 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>39</v>
@@ -12125,7 +12122,7 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>39</v>
@@ -12168,7 +12165,7 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>39</v>
@@ -12211,7 +12208,7 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>39</v>
@@ -12254,7 +12251,7 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>39</v>
@@ -12297,7 +12294,7 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>39</v>
@@ -12340,7 +12337,7 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>39</v>
@@ -12383,7 +12380,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>39</v>
@@ -12426,7 +12423,7 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>39</v>
@@ -12466,7 +12463,7 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>39</v>
@@ -12509,7 +12506,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>39</v>
@@ -12549,7 +12546,7 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>39</v>
@@ -12592,7 +12589,7 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>39</v>
@@ -12635,7 +12632,7 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>39</v>
@@ -12678,7 +12675,7 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>39</v>
@@ -12721,7 +12718,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>39</v>
@@ -12764,7 +12761,7 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>39</v>
@@ -12807,7 +12804,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>39</v>
@@ -12850,7 +12847,7 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>39</v>
@@ -12896,7 +12893,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>53</v>
@@ -12939,7 +12936,7 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>53</v>
@@ -12985,7 +12982,7 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>53</v>
@@ -13028,7 +13025,7 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>58</v>
@@ -13071,7 +13068,7 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>58</v>
@@ -13117,7 +13114,7 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>58</v>
@@ -13160,7 +13157,7 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>58</v>
@@ -13203,7 +13200,7 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>58</v>
@@ -13246,7 +13243,7 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>58</v>
@@ -13289,7 +13286,7 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>58</v>
@@ -13335,7 +13332,7 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>58</v>
@@ -13378,7 +13375,7 @@
     </row>
     <row r="186" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>67</v>
@@ -13418,7 +13415,7 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>67</v>
@@ -13461,7 +13458,7 @@
     </row>
     <row r="188" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>67</v>
@@ -13507,7 +13504,7 @@
     </row>
     <row r="189" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>67</v>
@@ -13547,7 +13544,7 @@
     </row>
     <row r="190" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>67</v>
@@ -13593,7 +13590,7 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>67</v>
@@ -13636,7 +13633,7 @@
     </row>
     <row r="192" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>67</v>
@@ -13682,7 +13679,7 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>67</v>
@@ -13725,7 +13722,7 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>67</v>
@@ -13768,7 +13765,7 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>67</v>
@@ -13811,7 +13808,7 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>67</v>
@@ -13854,7 +13851,7 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>67</v>
@@ -13897,7 +13894,7 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>67</v>
@@ -13940,7 +13937,7 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>67</v>
@@ -13983,7 +13980,7 @@
     </row>
     <row r="200" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>67</v>
@@ -14029,7 +14026,7 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>81</v>
@@ -14072,7 +14069,7 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>81</v>
@@ -14118,7 +14115,7 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>81</v>
@@ -14161,7 +14158,7 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>38</v>
+        <v>293</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>81</v>
@@ -14205,15 +14202,15 @@
   </sheetData>
   <autoFilter ref="A1:S204" xr:uid="{9210D030-08A6-47C5-BE1B-A368CD904E6C}"/>
   <conditionalFormatting sqref="A2:P204">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD($P2,2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J204">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>G2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>G2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14231,7 +14228,7 @@
   </sheetPr>
   <dimension ref="A1:C247"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>